<commit_message>
Fix: Corrigir cÃ¡lculo de credenciamentos na exportaÃ§Ã£o Excel
- Corrigido cÃ¡lculo de totalCredenciamentos na API excel-completo
- Alterado de f.credenciamentos.length para soma de qtdCredenciamentos
- Corrigido cÃ¡lculo no detalhamento por dia tambÃ©m
- Dados agora aparecem corretamente no Excel exportado
- Testado com dados reais: 30 credenciamentos totais
- Problema de dados zerados no Excel resolvido
</commit_message>
<xml_diff>
--- a/relatorio-completo-semanal-2025-10-23.xlsx
+++ b/relatorio-completo-semanal-2025-10-23.xlsx
@@ -4,7 +4,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
     <sheet name="Resumo Executivo" sheetId="1" r:id="rId1"/>
-    <sheet name="Cristian" sheetId="2" r:id="rId2"/>
+    <sheet name="Renan" sheetId="2" r:id="rId2"/>
     <sheet name="Análise Comparativa" sheetId="3" r:id="rId3"/>
     <sheet name="Cronograma Semanal" sheetId="4" r:id="rId4"/>
   </sheets>
@@ -439,7 +439,7 @@
         <v>Horário de Geração:</v>
       </c>
       <c r="B5" t="str">
-        <v>11:43:04</v>
+        <v>13:03:39</v>
       </c>
     </row>
     <row r="6">
@@ -457,7 +457,7 @@
         <v>Total de Credenciamentos:</v>
       </c>
       <c r="B8">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9">
@@ -465,7 +465,7 @@
         <v>Total de Volume R$:</v>
       </c>
       <c r="B9" t="str">
-        <v>R$ 20.725,33</v>
+        <v>R$ 73.491,33</v>
       </c>
     </row>
     <row r="10">
@@ -473,7 +473,7 @@
         <v>Total de Visitas:</v>
       </c>
       <c r="B10">
-        <v>18</v>
+        <v>52</v>
       </c>
     </row>
     <row r="11">
@@ -481,7 +481,7 @@
         <v>Total de Interações:</v>
       </c>
       <c r="B11">
-        <v>16</v>
+        <v>69</v>
       </c>
     </row>
     <row r="12">
@@ -489,7 +489,7 @@
         <v>Total Bra Expre:</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13">
@@ -564,46 +564,46 @@
     </row>
     <row r="18">
       <c r="A18" t="str">
-        <v>Cristian</v>
+        <v>Renan</v>
       </c>
       <c r="B18" t="str">
-        <v>Alegrete</v>
+        <v>AG 003 - Zona Norte</v>
       </c>
       <c r="C18">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="D18">
         <v>10</v>
       </c>
       <c r="E18" t="str">
-        <v>70.0%</v>
+        <v>160.0%</v>
       </c>
       <c r="F18" t="str">
-        <v>R$ 20.725,33</v>
+        <v>R$ 33.506,11</v>
       </c>
       <c r="G18" t="str">
         <v>R$ 150.000,00</v>
       </c>
       <c r="H18" t="str">
-        <v>13.8%</v>
+        <v>22.3%</v>
       </c>
       <c r="I18">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="J18">
         <v>30</v>
       </c>
       <c r="K18" t="str">
-        <v>60.0%</v>
+        <v>63.3%</v>
       </c>
       <c r="L18" t="str">
         <v>ABAIXO DA META</v>
       </c>
       <c r="M18">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="N18" t="str">
-        <v>100.0%</v>
+        <v>57.1%</v>
       </c>
     </row>
   </sheetData>
@@ -615,14 +615,14 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J37"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>📋 DETALHAMENTO COMPLETO - CRISTIAN</v>
+        <v>📋 DETALHAMENTO COMPLETO - RENAN</v>
       </c>
     </row>
     <row r="2">
@@ -630,7 +630,7 @@
         <v>Agência:</v>
       </c>
       <c r="B2" t="str">
-        <v>Alegrete</v>
+        <v>AG 003 - Zona Norte</v>
       </c>
     </row>
     <row r="3">
@@ -673,16 +673,16 @@
         <v>Credenciamentos</v>
       </c>
       <c r="B7">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="C7">
         <v>10</v>
       </c>
       <c r="D7" t="str">
-        <v>70.0%</v>
+        <v>160.0%</v>
       </c>
       <c r="E7" t="str">
-        <v>ABAIXO DA META</v>
+        <v>META BATIDA</v>
       </c>
     </row>
     <row r="8">
@@ -690,13 +690,13 @@
         <v>Volume (R$)</v>
       </c>
       <c r="B8" t="str">
-        <v>R$ 20.725,33</v>
+        <v>R$ 33.506,11</v>
       </c>
       <c r="C8" t="str">
         <v>R$ 150.000,00</v>
       </c>
       <c r="D8" t="str">
-        <v>13.8%</v>
+        <v>22.3%</v>
       </c>
       <c r="E8" t="str">
         <v>ABAIXO DA META</v>
@@ -707,13 +707,13 @@
         <v>Visitas</v>
       </c>
       <c r="B9">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C9">
         <v>30</v>
       </c>
       <c r="D9" t="str">
-        <v>60.0%</v>
+        <v>63.3%</v>
       </c>
       <c r="E9" t="str">
         <v>ABAIXO DA META</v>
@@ -734,7 +734,7 @@
         <v>Dias Trabalhados:</v>
       </c>
       <c r="B12">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="13">
@@ -742,7 +742,7 @@
         <v>Dias Esperados:</v>
       </c>
       <c r="B13">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14">
@@ -750,7 +750,7 @@
         <v>Percentual de Presença:</v>
       </c>
       <c r="B14" t="str">
-        <v>100.0%</v>
+        <v>57.1%</v>
       </c>
     </row>
     <row r="15">
@@ -758,7 +758,7 @@
         <v>Média Credenciamentos/Dia:</v>
       </c>
       <c r="B15" t="str">
-        <v>1.40</v>
+        <v>4.00</v>
       </c>
     </row>
     <row r="16">
@@ -766,7 +766,7 @@
         <v>Média Visitas/Dia:</v>
       </c>
       <c r="B16" t="str">
-        <v>3.60</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="17">
@@ -774,7 +774,7 @@
         <v>Total Interações:</v>
       </c>
       <c r="B17">
-        <v>16</v>
+        <v>22</v>
       </c>
     </row>
     <row r="18">
@@ -782,7 +782,7 @@
         <v>Total Bra Expre:</v>
       </c>
       <c r="B18">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -845,206 +845,134 @@
     </row>
     <row r="24">
       <c r="A24" t="str">
-        <v>19/10/2025</v>
-      </c>
-      <c r="B24" t="str">
-        <v>Segunda</v>
-      </c>
-      <c r="C24" t="str">
-        <v>Alegrete</v>
-      </c>
-      <c r="D24" t="str">
-        <v>5</v>
-      </c>
-      <c r="E24" t="str">
-        <v>4</v>
-      </c>
-      <c r="F24" t="str">
-        <v>2</v>
-      </c>
-      <c r="G24" t="str">
-        <v>1</v>
-      </c>
-      <c r="H24" t="str">
-        <v>R$ 5.000,00</v>
-      </c>
-      <c r="I24" t="str">
-        <v>0</v>
-      </c>
-      <c r="J24" t="str">
-        <v>R$ 0,00</v>
+        <v/>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="str">
-        <v/>
+        <v>📝 DETALHAMENTO COMPLETO DOS CREDENCIAMENTOS</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="str">
-        <v>📝 DETALHAMENTO COMPLETO DOS CREDENCIAMENTOS</v>
+        <v>Data</v>
+      </c>
+      <c r="B26" t="str">
+        <v>Dia da Semana</v>
+      </c>
+      <c r="C26" t="str">
+        <v>EC</v>
+      </c>
+      <c r="D26" t="str">
+        <v>Volume (R$)</v>
+      </c>
+      <c r="E26" t="str">
+        <v>RA</v>
+      </c>
+      <c r="F26" t="str">
+        <v>Qual Oferta?</v>
+      </c>
+      <c r="G26" t="str">
+        <v>Instala Direto</v>
+      </c>
+      <c r="H26" t="str">
+        <v>Gerente PJ</v>
+      </c>
+      <c r="I26" t="str">
+        <v>Horário</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="str">
-        <v>Data</v>
-      </c>
-      <c r="B27" t="str">
-        <v>Dia da Semana</v>
-      </c>
-      <c r="C27" t="str">
-        <v>EC</v>
-      </c>
-      <c r="D27" t="str">
-        <v>Volume (R$)</v>
-      </c>
-      <c r="E27" t="str">
-        <v>RA</v>
-      </c>
-      <c r="F27" t="str">
-        <v>Qual Oferta?</v>
-      </c>
-      <c r="G27" t="str">
-        <v>Instala Direto</v>
-      </c>
-      <c r="H27" t="str">
-        <v>Gerente PJ</v>
-      </c>
-      <c r="I27" t="str">
-        <v>Horário</v>
+        <v/>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="str">
-        <v>19/10/2025</v>
-      </c>
-      <c r="B28" t="str">
-        <v>Segunda</v>
-      </c>
-      <c r="C28" t="str">
-        <v>1234567890</v>
-      </c>
-      <c r="D28" t="str">
-        <v>R$ 5.000,00</v>
-      </c>
-      <c r="E28" t="str">
-        <v>Sim</v>
-      </c>
-      <c r="F28" t="str">
-        <v>Básica</v>
-      </c>
-      <c r="G28" t="str">
-        <v>Sim</v>
-      </c>
-      <c r="H28" t="str">
-        <v>João Silva</v>
-      </c>
-      <c r="I28" t="str">
-        <v>09:30:00</v>
+        <v>🔍 DETALHAMENTO COMPLETO DAS SIMULAÇÕES</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="str">
-        <v/>
+        <v>Data</v>
+      </c>
+      <c r="B29" t="str">
+        <v>Dia da Semana</v>
+      </c>
+      <c r="C29" t="str">
+        <v>CNPJ</v>
+      </c>
+      <c r="D29" t="str">
+        <v>Empresa</v>
+      </c>
+      <c r="E29" t="str">
+        <v>Faturamento (R$)</v>
+      </c>
+      <c r="F29" t="str">
+        <v>Comentários</v>
+      </c>
+      <c r="G29" t="str">
+        <v>Horário</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="str">
-        <v>🔍 DETALHAMENTO COMPLETO DAS SIMULAÇÕES</v>
+        <v/>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="str">
-        <v>Data</v>
-      </c>
-      <c r="B31" t="str">
-        <v>Dia da Semana</v>
-      </c>
-      <c r="C31" t="str">
-        <v>CNPJ</v>
-      </c>
-      <c r="D31" t="str">
-        <v>Empresa</v>
-      </c>
-      <c r="E31" t="str">
-        <v>Faturamento (R$)</v>
-      </c>
-      <c r="F31" t="str">
-        <v>Comentários</v>
-      </c>
-      <c r="G31" t="str">
-        <v>Horário</v>
+        <v>👥 ANÁLISE DOS GERENTES PJ</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="str">
-        <v/>
+        <v>Gerente PJ</v>
+      </c>
+      <c r="B32" t="str">
+        <v>Total Credenciamentos</v>
+      </c>
+      <c r="C32" t="str">
+        <v>Total Volume (R$)</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="str">
-        <v>👥 ANÁLISE DOS GERENTES PJ</v>
+        <v/>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="str">
-        <v>Gerente PJ</v>
-      </c>
-      <c r="B34" t="str">
-        <v>Total Credenciamentos</v>
-      </c>
-      <c r="C34" t="str">
-        <v>Total Volume (R$)</v>
+        <v>📊 RESUMO SEMANAL AVANÇADO</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="str">
-        <v>João Silva</v>
-      </c>
-      <c r="B35" t="str">
-        <v>1</v>
-      </c>
-      <c r="C35" t="str">
-        <v>R$ 5.000,00</v>
+        <v>Dias com Credenciamentos:</v>
+      </c>
+      <c r="B35">
+        <v>4</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="str">
-        <v/>
+        <v>Dias com Simulações:</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="str">
-        <v>📊 RESUMO SEMANAL AVANÇADO</v>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="str">
-        <v>Dias com Credenciamentos:</v>
-      </c>
-      <c r="B38">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="str">
-        <v>Dias com Simulações:</v>
-      </c>
-      <c r="B39">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="str">
         <v>Gerentes PJ Envolvidos:</v>
       </c>
-      <c r="B40" t="str">
-        <v>João Silva</v>
+      <c r="B37" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J40"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J37"/>
   </ignoredErrors>
 </worksheet>
 </file>
@@ -1110,25 +1038,25 @@
         <v>1</v>
       </c>
       <c r="B6" t="str">
-        <v>Cristian</v>
+        <v>Renan</v>
       </c>
       <c r="C6" t="str">
-        <v>Alegrete</v>
+        <v>AG 003 - Zona Norte</v>
       </c>
       <c r="D6" t="str">
-        <v>7</v>
+        <v>16</v>
       </c>
       <c r="E6" t="str">
         <v>10</v>
       </c>
       <c r="F6" t="str">
-        <v>70.0%</v>
+        <v>160.0%</v>
       </c>
       <c r="G6" t="str">
-        <v>ABAIXO DA META</v>
+        <v>META BATIDA</v>
       </c>
       <c r="H6" t="str">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7">
@@ -1172,25 +1100,25 @@
         <v>1</v>
       </c>
       <c r="B10" t="str">
-        <v>Cristian</v>
+        <v>Renan</v>
       </c>
       <c r="C10" t="str">
-        <v>Alegrete</v>
+        <v>AG 003 - Zona Norte</v>
       </c>
       <c r="D10" t="str">
-        <v>R$ 20.725,33</v>
+        <v>R$ 33.506,11</v>
       </c>
       <c r="E10" t="str">
         <v>R$ 150.000,00</v>
       </c>
       <c r="F10" t="str">
-        <v>13.8%</v>
+        <v>22.3%</v>
       </c>
       <c r="G10" t="str">
         <v>ABAIXO DA META</v>
       </c>
       <c r="H10" t="str">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="11">
@@ -1225,22 +1153,22 @@
     </row>
     <row r="14">
       <c r="A14" t="str">
-        <v>Cristian</v>
+        <v>Renan</v>
       </c>
       <c r="B14" t="str">
-        <v>Alegrete</v>
+        <v>AG 003 - Zona Norte</v>
       </c>
       <c r="C14" t="str">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D14" t="str">
-        <v>100.0%</v>
+        <v>57.1%</v>
       </c>
       <c r="E14" t="str">
-        <v>1.40</v>
+        <v>4.00</v>
       </c>
       <c r="F14" t="str">
-        <v>3.60</v>
+        <v>4.75</v>
       </c>
     </row>
   </sheetData>
@@ -1324,13 +1252,12 @@
         <v>Domingo</v>
       </c>
     </row>
-    <row r="6" xml:space="preserve">
+    <row r="6">
       <c r="A6" t="str">
-        <v>Cristian</v>
-      </c>
-      <c r="B6" t="str" xml:space="preserve">
-        <v xml:space="preserve">1 creds
-5 visitas</v>
+        <v>Renan</v>
+      </c>
+      <c r="B6" t="str">
+        <v>-</v>
       </c>
       <c r="C6" t="str">
         <v>-</v>

</xml_diff>